<commit_message>
Completed FPGA Module Layout
</commit_message>
<xml_diff>
--- a/Hardware/FPGA/DDR4 Pinouts.xlsx
+++ b/Hardware/FPGA/DDR4 Pinouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Desktop/Projects/DICE/Hardware/FPGA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0192E39A-B696-A149-8657-C943E0475A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767DDA21-A073-904B-88C6-06B67E455C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-8780" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{EC8C756A-D3D5-E94E-95C7-40C596DF75F8}"/>
   </bookViews>
@@ -2593,8 +2593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392156B9-7B8F-1848-8FD8-299C776CDEC9}">
   <dimension ref="A1:AK61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D56" workbookViewId="0">
-      <selection activeCell="AN95" sqref="AN95"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="75" workbookViewId="0">
+      <selection activeCell="AL52" sqref="AL52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>